<commit_message>
2023 July 11 12:07pm
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
+++ b/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
@@ -458,11 +458,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1058</v>
+        <v>0.1327</v>
       </c>
     </row>
     <row r="3">
@@ -473,11 +473,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0143</v>
+        <v>0.2366</v>
       </c>
     </row>
     <row r="4">
@@ -488,11 +488,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>bank</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.1327</v>
+        <v>-0.1438</v>
       </c>
     </row>
     <row r="5">
@@ -533,11 +533,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>bank</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.5286999999999999</v>
+        <v>-0.2167</v>
       </c>
     </row>
     <row r="8">
@@ -548,11 +548,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.2252</v>
+        <v>-0.5286999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +563,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.6975</v>
+        <v>-0.1311</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +578,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.1311</v>
+        <v>0.1349</v>
       </c>
     </row>
     <row r="11">
@@ -608,11 +608,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>credit</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5772</v>
+        <v>-0.4083</v>
       </c>
     </row>
     <row r="13">
@@ -623,11 +623,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.4083</v>
+        <v>0.8954</v>
       </c>
     </row>
     <row r="14">
@@ -638,11 +638,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>bank</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.865</v>
+        <v>-0.2377</v>
       </c>
     </row>
     <row r="15">
@@ -683,11 +683,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>bank</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.643</v>
+        <v>0.1918</v>
       </c>
     </row>
     <row r="18">
@@ -698,11 +698,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5832000000000001</v>
+        <v>-0.1808</v>
       </c>
     </row>
     <row r="19">
@@ -713,11 +713,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.7486</v>
+        <v>0.5832000000000001</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
2023 July 16 07:10pm
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
+++ b/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
@@ -458,11 +458,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1327</v>
+        <v>-0.6263</v>
       </c>
     </row>
     <row r="3">
@@ -488,11 +488,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bank</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.1438</v>
+        <v>0.08019999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -533,11 +533,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>bank</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.2167</v>
+        <v>-0.1311</v>
       </c>
     </row>
     <row r="8">
@@ -548,11 +548,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.5286999999999999</v>
+        <v>0.1349</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +563,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.1311</v>
+        <v>-0.4211</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +578,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.1349</v>
+        <v>-0.6423</v>
       </c>
     </row>
     <row r="11">
@@ -593,11 +593,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.4211</v>
+        <v>-0.0548</v>
       </c>
     </row>
     <row r="12">
@@ -608,11 +608,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.4083</v>
+        <v>0.8954</v>
       </c>
     </row>
     <row r="13">
@@ -623,11 +623,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.8954</v>
+        <v>-0.1748</v>
       </c>
     </row>
     <row r="14">
@@ -638,11 +638,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>bank</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.2377</v>
+        <v>0.4966</v>
       </c>
     </row>
     <row r="15">
@@ -653,11 +653,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.4966</v>
+        <v>0.4175</v>
       </c>
     </row>
     <row r="16">
@@ -683,11 +683,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>bank</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.1918</v>
+        <v>-0.1808</v>
       </c>
     </row>
     <row r="18">
@@ -698,11 +698,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.1808</v>
+        <v>0.5832000000000001</v>
       </c>
     </row>
     <row r="19">
@@ -713,11 +713,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.5832000000000001</v>
+        <v>0.8001</v>
       </c>
     </row>
     <row r="20">
@@ -728,11 +728,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>credit</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.4103</v>
+        <v>-0.1405</v>
       </c>
     </row>
     <row r="21">
@@ -743,11 +743,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.8001</v>
+        <v>-0.2575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 July 17 05:13pm
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
+++ b/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
@@ -473,11 +473,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2366</v>
+        <v>0.08019999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -488,11 +488,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.08019999999999999</v>
+        <v>-0.0263</v>
       </c>
     </row>
     <row r="5">
@@ -503,11 +503,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.0263</v>
+        <v>-0.2366</v>
       </c>
     </row>
     <row r="6">
@@ -518,11 +518,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.2366</v>
+        <v>-0.0926</v>
       </c>
     </row>
     <row r="7">
@@ -548,11 +548,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1349</v>
+        <v>-0.4211</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +563,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.4211</v>
+        <v>-0.6423</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +578,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.6423</v>
+        <v>-0.0548</v>
       </c>
     </row>
     <row r="11">
@@ -593,11 +593,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>invest</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.0548</v>
+        <v>-0.469</v>
       </c>
     </row>
     <row r="12">
@@ -608,11 +608,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.8954</v>
+        <v>-0.1748</v>
       </c>
     </row>
     <row r="13">
@@ -623,11 +623,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.1748</v>
+        <v>0.4966</v>
       </c>
     </row>
     <row r="14">
@@ -638,11 +638,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.4966</v>
+        <v>0.0533</v>
       </c>
     </row>
     <row r="15">
@@ -683,11 +683,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.1808</v>
+        <v>0.5832000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -698,11 +698,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5832000000000001</v>
+        <v>0.8001</v>
       </c>
     </row>
     <row r="19">
@@ -713,11 +713,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.8001</v>
+        <v>-0.1405</v>
       </c>
     </row>
     <row r="20">
@@ -728,11 +728,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>invest</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.1405</v>
+        <v>0.6494</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
2023 July 21 12:41pm
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
+++ b/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.0263</v>
+        <v>-0.0349</v>
       </c>
     </row>
     <row r="5">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.0926</v>
+        <v>-0.2623</v>
       </c>
     </row>
     <row r="7">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0533</v>
+        <v>0.0982</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.4175</v>
+        <v>0.4627</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.7827</v>
+        <v>0.7745</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.5832000000000001</v>
+        <v>0.5919</v>
       </c>
     </row>
     <row r="18">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.1405</v>
+        <v>-0.0626</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.6494</v>
+        <v>0.6402</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
Adjusting period ranges for the four models
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
+++ b/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
@@ -453,67 +453,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2006_2007</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>invest</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.6263</v>
+        <v>-0.1311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2006_2007</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.08019999999999999</v>
+        <v>-0.4211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2006_2007</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.0349</v>
+        <v>-0.6423</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2006_2007</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.2366</v>
+        <v>-0.0548</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2006_2007</t>
+          <t>2008_2009</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -522,28 +522,28 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.2623</v>
+        <v>-0.469</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.1311</v>
+        <v>-0.1748</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -552,28 +552,28 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.4211</v>
+        <v>0.4966</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.6423</v>
+        <v>0.0982</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -582,43 +582,43 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.0548</v>
+        <v>0.4627</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2010_2019</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.469</v>
+        <v>0.7745</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2020_2021</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>inflation</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.1748</v>
+        <v>0.1819</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2020_2021</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -627,58 +627,58 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.4966</v>
+        <v>0.2283</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2020_2021</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0982</v>
+        <v>0.7060999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2020_2021</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>invest</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.4627</v>
+        <v>-0.1322</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2020_2021</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>inflation</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.7745</v>
+        <v>-0.1933</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2020_2023</t>
+          <t>2022_2023</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -687,13 +687,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.5919</v>
+        <v>0.0525</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2020_2023</t>
+          <t>2022_2023</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -702,52 +702,52 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.8001</v>
+        <v>0.6238</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2020_2023</t>
+          <t>2022_2023</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>invest</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.0626</v>
+        <v>-0.1727</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2020_2023</t>
+          <t>2022_2023</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.6402</v>
+        <v>-0.5367</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2020_2023</t>
+          <t>2022_2023</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.2575</v>
+        <v>0.0973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed string int error
</commit_message>
<xml_diff>
--- a/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
+++ b/Models/Fed Models/Four Models/Correlation Table/Correlation Table Fed Funds.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2007-12_2009-06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2007-12_2009-06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -483,7 +483,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2007-12_2009-06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2007-12_2009-06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2008_2009</t>
+          <t>2007-12_2009-06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2009-07_2019-12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -543,7 +543,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2009-07_2019-12</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2009-07_2019-12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -573,7 +573,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2009-07_2019-12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2010_2019</t>
+          <t>2009-07_2019-12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -603,7 +603,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2020-01_2022-05</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -612,73 +612,73 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1819</v>
+        <v>0.821</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2020-01_2022-05</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>interest</t>
+          <t>uncertain</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.2283</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2020-01_2022-05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>invest</t>
+          <t>interest</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.7060999999999999</v>
+        <v>0.8708</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2020-01_2022-05</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>trade</t>
+          <t>invest</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.1322</v>
+        <v>0.1018</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2020_2021</t>
+          <t>2020-01_2022-05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>uncertain</t>
+          <t>trade</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.1933</v>
+        <v>0.706</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2022-06_2023-12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -687,13 +687,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.0525</v>
+        <v>-0.8116</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2022-06_2023-12</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6238</v>
+        <v>-0.2116</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2022-06_2023-12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.1727</v>
+        <v>0.2492</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2022-06_2023-12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -732,13 +732,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.5367</v>
+        <v>0.6523</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2022_2023</t>
+          <t>2022-06_2023-12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0973</v>
+        <v>0.4977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>